<commit_message>
Remove round status field and implement competition-level locking
- Remove status field from round table schema and all references
- Update all APIs to remove round status validation and queries
- Remove lock-unlock-round API (disabled, replaced with competition-level)
- Add new lock-unlock-competition API for LOCKED/UNLOCKED status
- Update frontend Competition.jsx with lock/unlock button for organisers
- Simplify game logic to use competition-level control instead of round-level
- Maintain security with organiser-only access and audit logging

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/LMS-Status-Flow.xlsx
+++ b/docs/LMS-Status-Flow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserPC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lmslocal2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76C03DE-4D76-4F9D-8083-810BC87F558A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCBB620-5A35-4294-9FF1-BC0FD91E4336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91A4C4BC-58E6-41D5-8658-97BC833B1072}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Lock time arrives or all choices made</t>
   </si>
@@ -65,33 +65,18 @@
     <t>Applying results</t>
   </si>
   <si>
-    <t>OPEN</t>
-  </si>
-  <si>
-    <t>CLOSE</t>
-  </si>
-  <si>
     <t>ADMIN ACTION</t>
   </si>
   <si>
     <t>ROUND TASK FLOW</t>
   </si>
   <si>
-    <t>CLOSED</t>
-  </si>
-  <si>
     <t>Players make their choices</t>
   </si>
   <si>
     <t>----</t>
   </si>
   <si>
-    <t>ROUND STATUS</t>
-  </si>
-  <si>
-    <t>COMPLETE</t>
-  </si>
-  <si>
     <t>MANUAL / AUTO</t>
   </si>
   <si>
@@ -101,22 +86,16 @@
     <t>COMPETITION STATUS</t>
   </si>
   <si>
-    <t>Admin can</t>
-  </si>
-  <si>
-    <t>DRAW</t>
-  </si>
-  <si>
-    <t>WINNER</t>
-  </si>
-  <si>
-    <t>Re-Open</t>
-  </si>
-  <si>
-    <t>CANCEL</t>
-  </si>
-  <si>
-    <t>Cancel</t>
+    <t>LOCKED</t>
+  </si>
+  <si>
+    <t>READY</t>
+  </si>
+  <si>
+    <t>UNLOCK</t>
+  </si>
+  <si>
+    <t>LOCK</t>
   </si>
 </sst>
 </file>
@@ -173,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,9 +171,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CD508B-0973-4E5C-8BA8-1F5E38010412}">
-  <dimension ref="B2:G22"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,16 +522,16 @@
   <sheetData>
     <row r="2" spans="2:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -563,10 +539,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
@@ -574,24 +550,24 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
@@ -602,13 +578,13 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
@@ -616,13 +592,13 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>2</v>
@@ -630,38 +606,38 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
@@ -675,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>2</v>
@@ -686,16 +662,16 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -703,48 +679,6 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>